<commit_message>
Updated Excel reports with test case data file
</commit_message>
<xml_diff>
--- a/NopCommerce/TestBase/TC_AddToCartTest_Report.xlsx
+++ b/NopCommerce/TestBase/TC_AddToCartTest_Report.xlsx
@@ -1,111 +1,59 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <definedNames/>
+  <calcPr calcId="122211" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Test Case ID</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Expected Result</t>
-  </si>
-  <si>
-    <t>Actual Result (After Execution)</t>
-  </si>
-  <si>
-    <t>Pass/Fail</t>
-  </si>
-  <si>
-    <t>Comments (Optional)</t>
-  </si>
-  <si>
-    <t>TC_01</t>
-  </si>
-  <si>
-    <t>TC_02</t>
-  </si>
-  <si>
-    <t>TC_03</t>
-  </si>
-  <si>
-    <t>TC_04</t>
-  </si>
-  <si>
-    <t>Add all items with random amounts</t>
-  </si>
-  <si>
-    <t>Check cart updates</t>
-  </si>
-  <si>
-    <t>Pick random item, search for it and then add it to cart</t>
-  </si>
-  <si>
-    <t>Multiple clicks on add to cart for an amount other than 1</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="5">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="0"/>
+      <sz val="13"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color theme="0"/>
+      <sz val="13"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Inherit"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -118,7 +66,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
+        <fgColor theme="3" tint="0.3999755851924192"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -152,40 +100,99 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -475,112 +482,148 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="33" customWidth="1"/>
-    <col min="6" max="6" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="61" customWidth="1"/>
+    <col width="15.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="31.140625" customWidth="1" min="2" max="2"/>
+    <col width="29.7109375" customWidth="1" min="3" max="3"/>
+    <col width="21.85546875" customWidth="1" min="4" max="4"/>
+    <col width="33" customWidth="1" min="5" max="5"/>
+    <col width="36.7109375" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="13.140625" customWidth="1" min="7" max="7"/>
+    <col width="61" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
+    <row r="1" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Test Case ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Password</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Expected Result</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Actual Result (After Execution)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Pass/Fail</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Comments (Optional)</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="33.75" thickBot="1">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+    <row r="2" ht="33.75" customHeight="1" thickBot="1">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>TC_01</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Add all items with random amounts</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="n"/>
+      <c r="D2" s="4" t="n"/>
+      <c r="E2" s="4" t="n"/>
+      <c r="F2" s="4" t="n"/>
+      <c r="G2" s="4" t="n"/>
+      <c r="H2" s="4" t="n"/>
     </row>
-    <row r="3" spans="1:8" ht="33.75" thickBot="1">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+    <row r="3" ht="33.75" customHeight="1" thickBot="1">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>TC_02</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Pick random item, search for it and then add it to cart</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="4" t="n"/>
+      <c r="E3" s="5" t="n"/>
+      <c r="F3" s="4" t="n"/>
+      <c r="G3" s="4" t="n"/>
+      <c r="H3" s="4" t="n"/>
     </row>
-    <row r="4" spans="1:8" ht="50.25" thickBot="1">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+    <row r="4" ht="50.25" customHeight="1" thickBot="1">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>TC_03</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Multiple clicks on add to cart for an amount other than 1</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n"/>
+      <c r="D4" s="4" t="n"/>
+      <c r="E4" s="5" t="n"/>
+      <c r="F4" s="4" t="n"/>
+      <c r="G4" s="4" t="n"/>
+      <c r="H4" s="4" t="n"/>
     </row>
-    <row r="5" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+    <row r="5" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>TC_04</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Check cart updates</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="n"/>
+      <c r="D5" s="4" t="n"/>
+      <c r="E5" s="5" t="n"/>
+      <c r="F5" s="4" t="n"/>
+      <c r="G5" s="4" t="n"/>
+      <c r="H5" s="4" t="n"/>
     </row>
-    <row r="15" spans="1:8">
-      <c r="E15" s="6"/>
+    <row r="15">
+      <c r="E15" s="6" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>